<commit_message>
bug all fixed for get_dash
</commit_message>
<xml_diff>
--- a/get_dash/budget.xlsx
+++ b/get_dash/budget.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,68 +434,43 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>budget</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>amount</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>userId</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>food</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>50</v>
+        <v>3000</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2020-1-20</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>ntu004</t>
+          <t>Dixon3220</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>food</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="C3" t="inlineStr">
-        <is>
-          <t>2020-3-1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
         <is>
           <t>ntu003</t>
         </is>
       </c>
     </row>
-    <row r="4"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
new_user window added to get_dash folder
</commit_message>
<xml_diff>
--- a/get_dash/budget.xlsx
+++ b/get_dash/budget.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,10 +436,30 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>budget</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>userId</t>
         </is>
@@ -450,9 +470,21 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
         <v>3000</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -463,11 +495,103 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
         <v>400</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>ntu003</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.18283207537334212</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.9025862388675534</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>3000</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.1105236658581672</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.09698904686853815</t>
         </is>
       </c>
     </row>

</xml_diff>